<commit_message>
database has been updated with availability of dog breed in India
</commit_message>
<xml_diff>
--- a/data/dogbreeddata.xlsx
+++ b/data/dogbreeddata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AksV\Desktop\Coding\git_lessons\PawPal\pawpal\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A684F69D-37DF-447B-BD07-49C1816F05FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3258535D-205C-46A0-82B8-D1A8B1748CA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7071" uniqueCount="559">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3625" uniqueCount="559">
   <si>
     <t>BreedName</t>
   </si>
@@ -2539,7 +2539,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q229"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D122" sqref="D122"/>
     </sheetView>
   </sheetViews>

</xml_diff>